<commit_message>
Se reemplazó el formato de comité tutor de Maestría
</commit_message>
<xml_diff>
--- a/assets/formatos/maestria/propuesta_comite_tutor_maestria.xlsx
+++ b/assets/formatos/maestria/propuesta_comite_tutor_maestria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sostenibilidad/Google Drive/Implantación PCS/Formatos Posgrado/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sostenibilidad UNAM\Google Drive\Implantación PCS\Formatos Posgrado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D5A34A-BD17-1A46-B325-88553EE259DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80859C8-B8AC-4C69-AE6F-80C778B79A0E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41840" yWindow="1140" windowWidth="34080" windowHeight="21960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31845" yWindow="3645" windowWidth="26325" windowHeight="14925" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
     <t>Especificar si está acreditado(a) en el Posgrado y anotar su adscripción</t>
   </si>
   <si>
-    <t>NOTA: NO SE REVISARÁN FORMATOS CON INFORMACIÓN INCOMPLETA.                                                                LAS PERSONAS PROPUESTAS PARA FORMAR PARTE DEL COMITÉ TUTOR QUE NO ESTÉN ACREDITADAS EN EL POSGRADO, PODRÁN SOLICITAR SU ACREDITACIÓN INGRESANDO A: https://sostenibilidad.posgrado.unam.mx/siges/accounts/signup/                                                                                   UNA VEZ INGRESANDO AL SISTEMA SERÁ NECESARIO REGISTRAR NOMBRE DE USUARIO, CONTRASEÑA Y CORREO ELECTRÓNICO. ES REQUISITO COMPLETAR EL FORMULARIO EN EL SISTEMA PARA QUE PROCEDA LA SOLICITUD DE ACREDITACIÓN.</t>
+    <t xml:space="preserve">NOTA: NO SE REVISARÁN FORMATOS CON INFORMACIÓN INCOMPLETA.                                                                </t>
   </si>
 </sst>
 </file>
@@ -201,6 +201,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -225,17 +231,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -675,94 +675,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AJ23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="231" zoomScaleNormal="135" zoomScalePageLayoutView="135" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:AJ23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="231" zoomScaleNormal="135" zoomScalePageLayoutView="135" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="44" width="2.33203125" style="2" customWidth="1"/>
-    <col min="45" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="44" width="2.375" style="2" customWidth="1"/>
+    <col min="45" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:36" ht="31" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="4" spans="1:36" ht="11" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="5" spans="1:36" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+    <row r="3" spans="1:36" ht="30.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:36" ht="11.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="5"/>
-      <c r="AG5" s="5"/>
-      <c r="AH5" s="5"/>
-      <c r="AI5" s="5"/>
-      <c r="AJ5" s="5"/>
-    </row>
-    <row r="7" spans="1:36" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="6"/>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="6"/>
-      <c r="AE7" s="6"/>
-      <c r="AF7" s="6"/>
-      <c r="AG7" s="6"/>
-      <c r="AH7" s="6"/>
-      <c r="AI7" s="6"/>
-      <c r="AJ7" s="6"/>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.15">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="9"/>
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="9"/>
+      <c r="AI5" s="9"/>
+      <c r="AJ5" s="9"/>
+    </row>
+    <row r="7" spans="1:36" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="10"/>
+      <c r="AE7" s="10"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="10"/>
+      <c r="AI7" s="10"/>
+      <c r="AJ7" s="10"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -776,340 +776,340 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.15">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="4"/>
-      <c r="Z10" s="4"/>
-      <c r="AA10" s="4"/>
-      <c r="AB10" s="4"/>
-      <c r="AC10" s="4"/>
-      <c r="AD10" s="4"/>
-      <c r="AE10" s="4"/>
-      <c r="AF10" s="4"/>
-      <c r="AG10" s="4"/>
-      <c r="AH10" s="4"/>
-      <c r="AI10" s="4"/>
-      <c r="AJ10" s="4"/>
-    </row>
-    <row r="11" spans="1:36" ht="53" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="8"/>
-      <c r="AB11" s="8"/>
-      <c r="AC11" s="8"/>
-      <c r="AD11" s="8"/>
-      <c r="AE11" s="8"/>
-      <c r="AF11" s="8"/>
-      <c r="AG11" s="8"/>
-      <c r="AH11" s="8"/>
-      <c r="AI11" s="8"/>
-      <c r="AJ11" s="9"/>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.15">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="8"/>
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="8"/>
+      <c r="AG10" s="8"/>
+      <c r="AH10" s="8"/>
+      <c r="AI10" s="8"/>
+      <c r="AJ10" s="8"/>
+    </row>
+    <row r="11" spans="1:36" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="12"/>
+      <c r="AD11" s="12"/>
+      <c r="AE11" s="12"/>
+      <c r="AF11" s="12"/>
+      <c r="AG11" s="12"/>
+      <c r="AH11" s="12"/>
+      <c r="AI11" s="12"/>
+      <c r="AJ11" s="13"/>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="11"/>
-      <c r="AB13" s="11"/>
-      <c r="AC13" s="11"/>
-      <c r="AD13" s="11"/>
-      <c r="AE13" s="11"/>
-      <c r="AF13" s="11"/>
-      <c r="AG13" s="11"/>
-      <c r="AH13" s="11"/>
-      <c r="AI13" s="11"/>
-      <c r="AJ13" s="11"/>
-    </row>
-    <row r="14" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="10"/>
-      <c r="Y14" s="10"/>
-      <c r="Z14" s="10"/>
-      <c r="AA14" s="10"/>
-      <c r="AB14" s="10"/>
-      <c r="AC14" s="10"/>
-      <c r="AD14" s="10"/>
-      <c r="AE14" s="10"/>
-      <c r="AF14" s="10"/>
-      <c r="AG14" s="10"/>
-      <c r="AH14" s="10"/>
-      <c r="AI14" s="10"/>
-      <c r="AJ14" s="10"/>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.15">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
+      <c r="V13" s="16"/>
+      <c r="W13" s="16"/>
+      <c r="X13" s="16"/>
+      <c r="Y13" s="16"/>
+      <c r="Z13" s="16"/>
+      <c r="AA13" s="16"/>
+      <c r="AB13" s="16"/>
+      <c r="AC13" s="16"/>
+      <c r="AD13" s="16"/>
+      <c r="AE13" s="16"/>
+      <c r="AF13" s="16"/>
+      <c r="AG13" s="16"/>
+      <c r="AH13" s="16"/>
+      <c r="AI13" s="16"/>
+      <c r="AJ13" s="16"/>
+    </row>
+    <row r="14" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="14"/>
+      <c r="AA14" s="14"/>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="14"/>
+      <c r="AD14" s="14"/>
+      <c r="AE14" s="14"/>
+      <c r="AF14" s="14"/>
+      <c r="AG14" s="14"/>
+      <c r="AH14" s="14"/>
+      <c r="AI14" s="14"/>
+      <c r="AJ14" s="14"/>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="P15" s="13" t="s">
+      <c r="P15" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="13" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="17" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="12" t="s">
+    <row r="16" spans="1:36" ht="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="P17" s="14" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="P17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="12"/>
-      <c r="V17" s="12"/>
-      <c r="W17" s="12"/>
-      <c r="X17" s="12"/>
-      <c r="Y17" s="12"/>
-      <c r="Z17" s="12"/>
-      <c r="AA17" s="12"/>
-      <c r="AB17" s="12"/>
-      <c r="AC17" s="12"/>
-      <c r="AD17" s="12"/>
-      <c r="AE17" s="12"/>
-      <c r="AF17" s="12"/>
-      <c r="AG17" s="12"/>
-      <c r="AH17" s="12"/>
-      <c r="AI17" s="12"/>
-      <c r="AJ17" s="12"/>
-    </row>
-    <row r="18" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="10"/>
-      <c r="Y18" s="10"/>
-      <c r="Z18" s="10"/>
-      <c r="AA18" s="10"/>
-      <c r="AB18" s="10"/>
-      <c r="AC18" s="10"/>
-      <c r="AD18" s="10"/>
-      <c r="AE18" s="10"/>
-      <c r="AF18" s="10"/>
-      <c r="AG18" s="10"/>
-      <c r="AH18" s="10"/>
-      <c r="AI18" s="10"/>
-      <c r="AJ18" s="10"/>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.15">
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
+      <c r="AG17" s="3"/>
+      <c r="AH17" s="3"/>
+      <c r="AI17" s="3"/>
+      <c r="AJ17" s="3"/>
+    </row>
+    <row r="18" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="14"/>
+      <c r="Y18" s="14"/>
+      <c r="Z18" s="14"/>
+      <c r="AA18" s="14"/>
+      <c r="AB18" s="14"/>
+      <c r="AC18" s="14"/>
+      <c r="AD18" s="14"/>
+      <c r="AE18" s="14"/>
+      <c r="AF18" s="14"/>
+      <c r="AG18" s="14"/>
+      <c r="AH18" s="14"/>
+      <c r="AI18" s="14"/>
+      <c r="AJ18" s="14"/>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P19" s="13" t="s">
+      <c r="P19" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
-      <c r="W20" s="10"/>
-      <c r="X20" s="10"/>
-      <c r="Y20" s="10"/>
-      <c r="Z20" s="10"/>
-      <c r="AA20" s="10"/>
-      <c r="AB20" s="10"/>
-      <c r="AC20" s="10"/>
-      <c r="AD20" s="10"/>
-      <c r="AE20" s="10"/>
-      <c r="AF20" s="10"/>
-      <c r="AG20" s="10"/>
-      <c r="AH20" s="10"/>
-      <c r="AI20" s="10"/>
-      <c r="AJ20" s="10"/>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:36" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="14"/>
+      <c r="W20" s="14"/>
+      <c r="X20" s="14"/>
+      <c r="Y20" s="14"/>
+      <c r="Z20" s="14"/>
+      <c r="AA20" s="14"/>
+      <c r="AB20" s="14"/>
+      <c r="AC20" s="14"/>
+      <c r="AD20" s="14"/>
+      <c r="AE20" s="14"/>
+      <c r="AF20" s="14"/>
+      <c r="AG20" s="14"/>
+      <c r="AH20" s="14"/>
+      <c r="AI20" s="14"/>
+      <c r="AJ20" s="14"/>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P21" s="13" t="s">
+      <c r="P21" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:36" ht="90" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="16" t="s">
+    <row r="23" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
-      <c r="W23" s="3"/>
-      <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
-      <c r="Z23" s="3"/>
-      <c r="AA23" s="3"/>
-      <c r="AB23" s="3"/>
-      <c r="AC23" s="3"/>
-      <c r="AD23" s="3"/>
-      <c r="AE23" s="3"/>
-      <c r="AF23" s="3"/>
-      <c r="AG23" s="3"/>
-      <c r="AH23" s="3"/>
-      <c r="AI23" s="3"/>
-      <c r="AJ23" s="3"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="7"/>
+      <c r="AC23" s="7"/>
+      <c r="AD23" s="7"/>
+      <c r="AE23" s="7"/>
+      <c r="AF23" s="7"/>
+      <c r="AG23" s="7"/>
+      <c r="AH23" s="7"/>
+      <c r="AI23" s="7"/>
+      <c r="AJ23" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>